<commit_message>
sprint demo prep PART 1
sprint demo prep PART 1
</commit_message>
<xml_diff>
--- a/cost register/netCamps_cost_register.xlsx
+++ b/cost register/netCamps_cost_register.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janfi\OneDrive\Pulpit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janfi\OneDrive\Dokumenty\GitHub\NetCamps\cost register\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{083168A8-24A5-4D5C-B177-83D533F35168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71399A72-DF3D-4A27-A7CB-37769406BC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{D9F21B02-6E43-49F3-9E63-1F2CCE1991A8}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>Product name</t>
   </si>
@@ -119,6 +119,42 @@
   <si>
     <t>Labour</t>
   </si>
+  <si>
+    <t>Cisco WS-C2960-24TT-L</t>
+  </si>
+  <si>
+    <t>Switch used for accessing and VLAN trunk links</t>
+  </si>
+  <si>
+    <t>Cisco CISCO2911/K9</t>
+  </si>
+  <si>
+    <t>Routers for backbone campus network</t>
+  </si>
+  <si>
+    <t>Lenovo ThinkPad P50</t>
+  </si>
+  <si>
+    <t>Admin computer next to DHCP server</t>
+  </si>
+  <si>
+    <t>DHCP server</t>
+  </si>
+  <si>
+    <t>ASR1002-5G/K9</t>
+  </si>
+  <si>
+    <t>Fiber</t>
+  </si>
+  <si>
+    <t>Backbone fiber cabling</t>
+  </si>
+  <si>
+    <t>Cooper</t>
+  </si>
+  <si>
+    <t>Ethernet cabling CAT 8</t>
+  </si>
 </sst>
 </file>
 
@@ -340,6 +376,1123 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>NetCamps cost summary</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$C$5:$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Routers</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Switches</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Servers</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Cables</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Computers</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Printers</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Phones</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>IoT equipment</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Labour</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$E$5:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3592</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3930</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5640</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1550</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BFC6-4785-AAF7-641BCFBE710E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1706985040"/>
+        <c:axId val="1708699264"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$C$5:$C$13</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>Routers</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Switches</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Servers</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Cables</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Computers</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Printers</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Phones</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>IoT equipment</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Labour</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$D$5:$D$13</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-BFC6-4785-AAF7-641BCFBE710E}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1706985040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Cost element</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.50149190726159232"/>
+              <c:y val="0.87405074365704283"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1708699264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1708699264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Total Cost [PLN]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1706985040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>11430</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>445770</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>156209</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCD32518-AF4D-8881-5788-250CC9DBF52C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -641,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963F0518-74EF-4808-AA9B-C3A46FB3F5EC}">
   <dimension ref="C3:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -671,7 +1824,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1">
         <f>Routers!H2</f>
-        <v>0</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.55000000000000004">
@@ -681,7 +1834,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1">
         <f>Switches!H2</f>
-        <v>0</v>
+        <v>3930</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.55000000000000004">
@@ -691,7 +1844,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1">
         <f>Servers!H2</f>
-        <v>0</v>
+        <v>898</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.55000000000000004">
@@ -701,7 +1854,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1">
         <f>Cables!H2</f>
-        <v>0</v>
+        <v>5640</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.55000000000000004">
@@ -711,7 +1864,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1">
         <f>Computers!H2</f>
-        <v>0</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.55000000000000004">
@@ -771,6 +1924,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -902,13 +2056,13 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="22.1015625" customWidth="1"/>
-    <col min="3" max="3" width="18.578125" customWidth="1"/>
+    <col min="3" max="3" width="31.41796875" customWidth="1"/>
     <col min="4" max="4" width="13.1015625" customWidth="1"/>
     <col min="5" max="5" width="10.89453125" customWidth="1"/>
     <col min="7" max="7" width="18.05078125" customWidth="1"/>
@@ -934,14 +2088,22 @@
       </c>
       <c r="H2" s="2" cm="1">
         <f t="array" ref="H2">SUM(D3:D200*E3:E200)</f>
-        <v>0</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1">
+        <v>898</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3"/>
@@ -1022,13 +2184,13 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="22.26171875" customWidth="1"/>
-    <col min="3" max="3" width="25.7890625" customWidth="1"/>
+    <col min="3" max="3" width="45.62890625" customWidth="1"/>
     <col min="4" max="4" width="24.734375" customWidth="1"/>
     <col min="5" max="5" width="31.7890625" customWidth="1"/>
     <col min="7" max="7" width="16.05078125" customWidth="1"/>
@@ -1053,14 +2215,22 @@
       </c>
       <c r="H2" s="2" cm="1">
         <f t="array" ref="H2">SUM(D3:D200*E3:E200)</f>
-        <v>0</v>
+        <v>3930</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
+        <v>655</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3"/>
@@ -1141,7 +2311,7 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1172,15 +2342,23 @@
         <v>4</v>
       </c>
       <c r="H2" s="2" cm="1">
-        <f t="array" ref="H2">SUM(E4:E201*F4:F201)</f>
-        <v>0</v>
+        <f t="array" ref="H2">SUM(D3:D201*E3:E201)</f>
+        <v>898</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1">
+        <v>898</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3"/>
@@ -1261,7 +2439,7 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1293,21 +2471,39 @@
         <v>4</v>
       </c>
       <c r="H2" s="2" cm="1">
-        <f t="array" ref="H2">SUM(E4:E201*F4:F201)</f>
-        <v>0</v>
+        <f t="array" ref="H2">SUM(D3:D201*E3:E201)</f>
+        <v>5640</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1">
+        <f>8*180</f>
+        <v>1440</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="3"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1">
+        <f>(20*90*6+20*90)/3</f>
+        <v>4200</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="3"/>
@@ -1382,13 +2578,13 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="17.26171875" customWidth="1"/>
-    <col min="3" max="3" width="21.68359375" customWidth="1"/>
+    <col min="2" max="2" width="19.41796875" customWidth="1"/>
+    <col min="3" max="3" width="30.3125" customWidth="1"/>
     <col min="4" max="4" width="18.20703125" customWidth="1"/>
     <col min="5" max="5" width="23.9453125" customWidth="1"/>
     <col min="7" max="7" width="20.734375" customWidth="1"/>
@@ -1413,15 +2609,23 @@
         <v>4</v>
       </c>
       <c r="H2" s="2" cm="1">
-        <f t="array" ref="H2">SUM(E4:E201*F4:F201)</f>
-        <v>0</v>
+        <f t="array" ref="H2">SUM(D3:D201*E3:E201)</f>
+        <v>1550</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1550</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3"/>

</xml_diff>

<commit_message>
Sprint DEMO final commit
</commit_message>
<xml_diff>
--- a/cost register/netCamps_cost_register.xlsx
+++ b/cost register/netCamps_cost_register.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janfi\OneDrive\Dokumenty\GitHub\NetCamps\cost register\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71399A72-DF3D-4A27-A7CB-37769406BC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D219F95B-F059-447B-A0D3-2DDD1C7DD4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{D9F21B02-6E43-49F3-9E63-1F2CCE1991A8}"/>
+    <workbookView xWindow="3780" yWindow="4200" windowWidth="28800" windowHeight="15460" activeTab="1" xr2:uid="{D9F21B02-6E43-49F3-9E63-1F2CCE1991A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="10" r:id="rId1"/>
     <sheet name="Routers" sheetId="1" r:id="rId2"/>
     <sheet name="Switches" sheetId="2" r:id="rId3"/>
     <sheet name="Servers" sheetId="8" r:id="rId4"/>
-    <sheet name="Cables" sheetId="4" r:id="rId5"/>
-    <sheet name="Computers" sheetId="5" r:id="rId6"/>
-    <sheet name="Printers" sheetId="6" r:id="rId7"/>
-    <sheet name="Phones" sheetId="7" r:id="rId8"/>
-    <sheet name="IoT" sheetId="3" r:id="rId9"/>
-    <sheet name="Labour" sheetId="9" r:id="rId10"/>
+    <sheet name="Wireless" sheetId="9" r:id="rId5"/>
+    <sheet name="Cables" sheetId="4" r:id="rId6"/>
+    <sheet name="Computers" sheetId="5" r:id="rId7"/>
+    <sheet name="Printers" sheetId="6" r:id="rId8"/>
+    <sheet name="Phones" sheetId="7" r:id="rId9"/>
+    <sheet name="IoT" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
   <si>
     <t>Product name</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Product type description</t>
   </si>
   <si>
-    <t>Total cost</t>
-  </si>
-  <si>
     <t>Routers</t>
   </si>
   <si>
@@ -117,18 +114,12 @@
     <t>IoT equipment</t>
   </si>
   <si>
-    <t>Labour</t>
-  </si>
-  <si>
     <t>Cisco WS-C2960-24TT-L</t>
   </si>
   <si>
     <t>Switch used for accessing and VLAN trunk links</t>
   </si>
   <si>
-    <t>Cisco CISCO2911/K9</t>
-  </si>
-  <si>
     <t>Routers for backbone campus network</t>
   </si>
   <si>
@@ -154,6 +145,24 @@
   </si>
   <si>
     <t>Ethernet cabling CAT 8</t>
+  </si>
+  <si>
+    <t>Cisco CP-7942G</t>
+  </si>
+  <si>
+    <t>IP phone produced by C</t>
+  </si>
+  <si>
+    <t>Wireless</t>
+  </si>
+  <si>
+    <t>SUMA</t>
+  </si>
+  <si>
+    <t>Total cost [PLN]</t>
+  </si>
+  <si>
+    <t>Cisco CISCO2811</t>
   </si>
 </sst>
 </file>
@@ -177,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +196,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -361,6 +376,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -470,7 +487,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Summary!$C$5:$C$13</c:f>
+              <c:f>Summary!$C$5:$C$14</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -498,37 +515,37 @@
                   <c:v>IoT equipment</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Labour</c:v>
+                  <c:v>Wireless</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$E$5:$E$13</c:f>
+              <c:f>Summary!$E$5:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3592</c:v>
+                  <c:v>34968</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3930</c:v>
+                  <c:v>6330</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>898</c:v>
+                  <c:v>18300</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5640</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1550</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>4500</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -578,7 +595,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$C$5:$C$13</c15:sqref>
+                          <c15:sqref>Summary!$C$5:$C$14</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -609,7 +626,7 @@
                         <c:v>IoT equipment</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>Labour</c:v>
+                        <c:v>Wireless</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -619,13 +636,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$D$5:$D$13</c15:sqref>
+                          <c15:sqref>Summary!$D$5:$D$14</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="9"/>
+                      <c:ptCount val="10"/>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -646,70 +663,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Cost element</a:t>
-                </a:r>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.50149190726159232"/>
-              <c:y val="0.87405074365704283"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1458,16 +1411,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>11430</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3174</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>445770</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>156209</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1792,21 +1745,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963F0518-74EF-4808-AA9B-C3A46FB3F5EC}">
-  <dimension ref="C3:E16"/>
+  <dimension ref="C3:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="17.89453125" customWidth="1"/>
-    <col min="4" max="4" width="28.41796875" customWidth="1"/>
-    <col min="5" max="5" width="22.1015625" customWidth="1"/>
+    <col min="3" max="3" width="17.90625" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" customWidth="1"/>
+    <col min="5" max="5" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1814,42 +1767,42 @@
         <v>6</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C5" s="11" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="11" t="s">
-        <v>8</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1">
         <f>Routers!H2</f>
-        <v>3592</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+        <v>34968</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C6" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1">
         <f>Switches!H2</f>
-        <v>3930</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+        <v>6330</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C7" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1">
         <f>Servers!H2</f>
-        <v>898</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+        <v>18300</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C8" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1">
@@ -1857,19 +1810,19 @@
         <v>5640</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C9" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1">
         <f>Computers!H2</f>
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C10" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
@@ -1877,19 +1830,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C11" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1">
         <f>Phones!H2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C12" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1">
@@ -1897,30 +1850,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C13" s="11" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1">
-        <f>Labour!H2</f>
+        <f>Wireless!H2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C14" s="3"/>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C14" s="11"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C15" s="3"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="3:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="12">
+        <f>SUM(E5:E16)</f>
+        <v>72138</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1929,28 +1892,28 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BCCE6A-D75E-4EE9-832E-46E5198DCED7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC0D58B-F441-489C-8D73-D11878634A6E}">
   <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
+    <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.20703125" customWidth="1"/>
-    <col min="3" max="3" width="22.47265625" customWidth="1"/>
-    <col min="4" max="4" width="23.734375" customWidth="1"/>
-    <col min="5" max="5" width="31.578125" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="32.47265625" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
+    <col min="4" max="4" width="28.81640625" customWidth="1"/>
+    <col min="5" max="5" width="32.1796875" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" customWidth="1"/>
+    <col min="8" max="8" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1971,73 +1934,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2055,22 +2018,22 @@
   </sheetPr>
   <dimension ref="B1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.1015625" customWidth="1"/>
-    <col min="3" max="3" width="31.41796875" customWidth="1"/>
-    <col min="4" max="4" width="13.1015625" customWidth="1"/>
-    <col min="5" max="5" width="10.89453125" customWidth="1"/>
-    <col min="7" max="7" width="18.05078125" customWidth="1"/>
-    <col min="8" max="8" width="8.83984375" customWidth="1"/>
+    <col min="2" max="2" width="22.08984375" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" customWidth="1"/>
+    <col min="7" max="7" width="18.08984375" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2088,84 +2051,84 @@
       </c>
       <c r="H2" s="2" cm="1">
         <f t="array" ref="H2">SUM(D3:D200*E3:E200)</f>
-        <v>3592</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>34968</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1">
-        <v>898</v>
+        <v>8742</v>
       </c>
       <c r="E3" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2184,20 +2147,20 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.26171875" customWidth="1"/>
-    <col min="3" max="3" width="45.62890625" customWidth="1"/>
-    <col min="4" max="4" width="24.734375" customWidth="1"/>
-    <col min="5" max="5" width="31.7890625" customWidth="1"/>
-    <col min="7" max="7" width="16.05078125" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" customWidth="1"/>
+    <col min="3" max="3" width="45.6328125" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" customWidth="1"/>
+    <col min="5" max="5" width="31.81640625" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2215,84 +2178,84 @@
       </c>
       <c r="H2" s="2" cm="1">
         <f t="array" ref="H2">SUM(D3:D200*E3:E200)</f>
-        <v>3930</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>6330</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1">
-        <v>655</v>
+        <v>1055</v>
       </c>
       <c r="E3" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2311,21 +2274,21 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.26171875" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.62890625" customWidth="1"/>
-    <col min="5" max="5" width="22.83984375" customWidth="1"/>
-    <col min="7" max="7" width="20.62890625" customWidth="1"/>
-    <col min="8" max="8" width="33.1015625" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" customWidth="1"/>
+    <col min="7" max="7" width="20.6328125" customWidth="1"/>
+    <col min="8" max="8" width="33.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2343,84 +2306,84 @@
       </c>
       <c r="H2" s="2" cm="1">
         <f t="array" ref="H2">SUM(D3:D201*E3:E201)</f>
-        <v>898</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>18300</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1">
-        <v>898</v>
+        <v>6100</v>
       </c>
       <c r="E3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2432,6 +2395,126 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BCCE6A-D75E-4EE9-832E-46E5198DCED7}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="B1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="23.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.453125" customWidth="1"/>
+    <col min="4" max="4" width="23.7265625" customWidth="1"/>
+    <col min="5" max="5" width="31.54296875" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="32.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" cm="1">
+        <f t="array" ref="H2">SUM(D3:D201*E3:E201)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="3"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="3"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="3"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="3"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="3"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="3"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="3"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="3"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="3"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="3"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5D59A5-0D18-4B26-B0D7-63A4E7A24585}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2439,22 +2522,22 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.15625" customWidth="1"/>
-    <col min="3" max="3" width="22.7890625" customWidth="1"/>
-    <col min="4" max="4" width="24.578125" customWidth="1"/>
-    <col min="5" max="5" width="29.5234375" customWidth="1"/>
-    <col min="6" max="6" width="19.734375" customWidth="1"/>
-    <col min="7" max="8" width="15.578125" customWidth="1"/>
-    <col min="9" max="9" width="19.15625" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
+    <col min="4" max="4" width="24.54296875" customWidth="1"/>
+    <col min="5" max="5" width="29.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.7265625" customWidth="1"/>
+    <col min="7" max="8" width="15.54296875" customWidth="1"/>
+    <col min="9" max="9" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2475,12 +2558,12 @@
         <v>5640</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1">
         <f>8*180</f>
@@ -2490,12 +2573,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1">
         <f>(20*90*6+20*90)/3</f>
@@ -2505,61 +2588,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2570,7 +2653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C250B418-17E0-4AB7-A260-B195AC84A536}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2578,21 +2661,21 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.41796875" customWidth="1"/>
-    <col min="3" max="3" width="30.3125" customWidth="1"/>
-    <col min="4" max="4" width="18.20703125" customWidth="1"/>
-    <col min="5" max="5" width="23.9453125" customWidth="1"/>
-    <col min="7" max="7" width="20.734375" customWidth="1"/>
-    <col min="8" max="8" width="26.26171875" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="3" max="3" width="30.26953125" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+    <col min="5" max="5" width="23.90625" customWidth="1"/>
+    <col min="7" max="7" width="20.7265625" customWidth="1"/>
+    <col min="8" max="8" width="26.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2610,84 +2693,84 @@
       </c>
       <c r="H2" s="2" cm="1">
         <f t="array" ref="H2">SUM(D3:D201*E3:E201)</f>
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1">
-        <v>1550</v>
+        <v>2400</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2698,7 +2781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E589B81-B94A-4B32-8658-CF08D05EDAA9}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2709,18 +2792,17 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.62890625" customWidth="1"/>
-    <col min="3" max="3" width="18.83984375" customWidth="1"/>
-    <col min="4" max="4" width="18.7890625" customWidth="1"/>
-    <col min="5" max="5" width="20.5234375" customWidth="1"/>
-    <col min="7" max="7" width="19.47265625" customWidth="1"/>
-    <col min="8" max="8" width="20.89453125" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" customWidth="1"/>
+    <col min="3" max="4" width="18.81640625" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" customWidth="1"/>
+    <col min="8" max="8" width="20.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2741,73 +2823,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2818,7 +2900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7755B782-31B1-476D-8190-D072F3C03FE8}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2826,21 +2908,21 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.1015625" customWidth="1"/>
-    <col min="3" max="3" width="20.62890625" customWidth="1"/>
-    <col min="4" max="4" width="22.7890625" customWidth="1"/>
-    <col min="5" max="5" width="26.3125" customWidth="1"/>
-    <col min="7" max="7" width="24.3671875" customWidth="1"/>
-    <col min="8" max="8" width="29.734375" customWidth="1"/>
+    <col min="2" max="2" width="19.08984375" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="26.26953125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="8" max="8" width="29.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2857,77 +2939,85 @@
         <v>4</v>
       </c>
       <c r="H2" s="2" cm="1">
-        <f t="array" ref="H2">SUM(E4:E201*F4:F201)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <f t="array" ref="H2">SUM(D3:D201*E3:E201)</f>
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1">
+        <v>150</v>
+      </c>
+      <c r="E3" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2936,124 +3026,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC0D58B-F441-489C-8D73-D11878634A6E}">
-  <sheetPr>
-    <tabColor rgb="FF92D050"/>
-  </sheetPr>
-  <dimension ref="B1:H14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="2" max="2" width="21.26171875" customWidth="1"/>
-    <col min="3" max="3" width="22.1015625" customWidth="1"/>
-    <col min="4" max="4" width="28.83984375" customWidth="1"/>
-    <col min="5" max="5" width="32.20703125" customWidth="1"/>
-    <col min="7" max="7" width="22.20703125" customWidth="1"/>
-    <col min="8" max="8" width="29" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="2" cm="1">
-        <f t="array" ref="H2">SUM(E4:E201*F4:F201)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="3"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="3"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="3"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="3"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="3"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="3"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="3"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="3"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="3"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="3"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
iot cost register update
iot cost register update
</commit_message>
<xml_diff>
--- a/cost register/netCamps_cost_register.xlsx
+++ b/cost register/netCamps_cost_register.xlsx
@@ -1,26 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janfi\OneDrive\Dokumenty\GitHub\NetCamps\cost register\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE95F3FF-B7D6-4FF1-9A53-CFA968F3E74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Summary" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Routers" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Switches" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Servers" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Wireless" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Cables" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Computers" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Printers" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="Phones" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="IoT" sheetId="10" r:id="rId13"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Routers" sheetId="2" r:id="rId2"/>
+    <sheet name="Switches" sheetId="3" r:id="rId3"/>
+    <sheet name="Servers" sheetId="4" r:id="rId4"/>
+    <sheet name="Wireless" sheetId="5" r:id="rId5"/>
+    <sheet name="Cables" sheetId="6" r:id="rId6"/>
+    <sheet name="Computers" sheetId="7" r:id="rId7"/>
+    <sheet name="Printers" sheetId="8" r:id="rId8"/>
+    <sheet name="Phones" sheetId="9" r:id="rId9"/>
+    <sheet name="IoT" sheetId="10" r:id="rId10"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
   <si>
     <t>Product type</t>
   </si>
@@ -186,49 +230,89 @@
   <si>
     <t>IP phone produced by C</t>
   </si>
+  <si>
+    <t>Linksys WRT 300N</t>
+  </si>
+  <si>
+    <t>Wireless Access Points for IoT</t>
+  </si>
+  <si>
+    <t>IoT lamp  E27</t>
+  </si>
+  <si>
+    <t>Iot Lamps for Dorms</t>
+  </si>
+  <si>
+    <t>CZUJNIK RUCHU STEINEL IS2360-3 ECO IP54</t>
+  </si>
+  <si>
+    <t>motion detector</t>
+  </si>
+  <si>
+    <t>TP-Link Tapo C500</t>
+  </si>
+  <si>
+    <t>Iot camera</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi Smart Standing Fan 2</t>
+  </si>
+  <si>
+    <t>iot fan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ [$zł-415]"/>
   </numFmts>
   <fonts count="7">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -237,7 +321,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -259,7 +343,13 @@
     </fill>
   </fills>
   <borders count="10">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
@@ -273,6 +363,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -287,6 +378,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -301,6 +393,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -315,6 +408,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -329,6 +423,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -343,6 +438,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -357,6 +453,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -371,6 +468,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -385,85 +483,74 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -472,7 +559,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0" i="0" sz="1400">
+              <a:defRPr sz="1400" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -480,7 +567,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" i="0" sz="1400">
+              <a:rPr lang="pl-PL" sz="1400" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -493,16 +580,19 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="ED7D31"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -510,18 +600,107 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
               <c:f>Summary!$C$5:$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Routers</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Switches</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Servers</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Cables</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Computers</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Printers</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Phones</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>IoT equipment</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Wireless</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Summary!$E$5:$E$14</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>#,##0\ [$zł-415]</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>34968</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6330</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14974.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10080</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                  <a:ln cmpd="sng">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-24CF-49AB-B7A4-EF4393B40437}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="129627401"/>
         <c:axId val="21392694"/>
       </c:barChart>
@@ -546,15 +725,7 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -563,22 +734,28 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0" i="0" sz="900">
+              <a:defRPr sz="900" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="21392694"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="21392694"/>
@@ -603,7 +780,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr lvl="0">
-                  <a:defRPr b="0" i="0" sz="1000">
+                  <a:defRPr sz="1000" b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -611,7 +788,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" i="0" sz="1000">
+                  <a:rPr lang="pl-PL" sz="1000" b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -624,7 +801,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0\ [$zł-415]" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -636,25 +813,35 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0" i="0" sz="900">
+              <a:defRPr sz="900" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="129627401"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -663,9 +850,15 @@
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6867525" cy="3962400"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1" title="Wykres"/>
+        <xdr:cNvPr id="2" name="Chart 1" title="Wykres">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -674,7 +867,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -683,44 +876,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -910,30 +1067,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="8.71"/>
-    <col customWidth="1" min="3" max="3" width="17.86"/>
-    <col customWidth="1" min="4" max="4" width="26.43"/>
-    <col customWidth="1" min="5" max="5" width="22.14"/>
-    <col customWidth="1" min="6" max="26" width="8.71"/>
+    <col min="1" max="2" width="8.68359375" customWidth="1"/>
+    <col min="3" max="3" width="17.83984375" customWidth="1"/>
+    <col min="4" max="4" width="26.41796875" customWidth="1"/>
+    <col min="5" max="5" width="22.15625" customWidth="1"/>
+    <col min="6" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1"/>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="1" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="2" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="3" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="4" spans="3:5" ht="14.25" customHeight="1">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -944,7 +1103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="3:5" ht="14.25" customHeight="1">
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
@@ -954,7 +1113,7 @@
         <v>34968</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="3:5" ht="14.25" customHeight="1">
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
@@ -964,7 +1123,7 @@
         <v>6330</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="3:5" ht="14.25" customHeight="1">
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
@@ -974,7 +1133,7 @@
         <v>20900</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="3:5" ht="14.25" customHeight="1">
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
@@ -984,7 +1143,7 @@
         <v>14974.8</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="3:5" ht="14.25" customHeight="1">
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
@@ -994,7 +1153,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="3:5" ht="14.25" customHeight="1">
       <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1004,7 +1163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="3:5" ht="14.25" customHeight="1">
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1014,17 +1173,17 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="3:5" ht="14.25" customHeight="1">
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="5">
         <f>IoT!H2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
+        <v>10080</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" ht="14.25" customHeight="1">
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1034,46 +1193,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="3:5" ht="14.25" customHeight="1">
       <c r="C14" s="3"/>
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="3:5" ht="14.25" customHeight="1">
       <c r="C15" s="6"/>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="3:5" ht="14.25" customHeight="1">
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="17" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="18" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="19" spans="3:5" ht="14.25" customHeight="1">
       <c r="C19" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="12">
         <f>SUM(E5:E16)</f>
-        <v>86772.8</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+        <v>96852.800000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="21" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="22" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="23" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="24" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="25" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="26" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="27" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="28" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="29" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="30" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="31" spans="3:5" ht="14.25" customHeight="1"/>
+    <row r="32" spans="3:5" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2043,37 +2202,38 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="21.29"/>
-    <col customWidth="1" min="3" max="3" width="22.14"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="29.0"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
-    <col customWidth="1" min="7" max="7" width="22.14"/>
-    <col customWidth="1" min="8" max="8" width="29.0"/>
-    <col customWidth="1" min="9" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="21.26171875" customWidth="1"/>
+    <col min="3" max="3" width="22.15625" customWidth="1"/>
+    <col min="4" max="4" width="28.83984375" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="8.68359375" customWidth="1"/>
+    <col min="7" max="7" width="22.15625" customWidth="1"/>
+    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="1" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="2" spans="2:8" ht="14.25" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -2089,85 +2249,125 @@
       <c r="G2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="14">
-        <f t="array" ref="H2">SUM(E4:E201*F4:F201)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="B3" s="6"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="17"/>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="B4" s="6"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="B5" s="6"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="B6" s="6"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
+      <c r="H2" s="14" cm="1">
+        <f t="array" ref="H2">SUM(D3:D201*E3:E201)</f>
+        <v>10080</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="14.25" customHeight="1">
+      <c r="B3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="4">
+        <v>300</v>
+      </c>
+      <c r="E3" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="14.25" customHeight="1">
+      <c r="B4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="4">
+        <v>300</v>
+      </c>
+      <c r="E4" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="14.25" customHeight="1">
+      <c r="B5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="4">
+        <v>300</v>
+      </c>
+      <c r="E5" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="14.25" customHeight="1">
+      <c r="B6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="4">
+        <v>200</v>
+      </c>
+      <c r="E6" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="14.25" customHeight="1">
+      <c r="B7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="4">
+        <v>530</v>
+      </c>
+      <c r="E7" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="14.25" customHeight="1">
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" ht="14.25" customHeight="1">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="14.25" customHeight="1">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.25" customHeight="1">
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:8" ht="14.25" customHeight="1">
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:8" ht="14.25" customHeight="1">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="16" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -3153,37 +3353,35 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="22.14"/>
-    <col customWidth="1" min="3" max="3" width="31.43"/>
-    <col customWidth="1" min="4" max="4" width="13.14"/>
-    <col customWidth="1" min="5" max="5" width="10.86"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
-    <col customWidth="1" min="7" max="7" width="18.14"/>
-    <col customWidth="1" min="8" max="8" width="8.86"/>
-    <col customWidth="1" min="9" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="22.15625" customWidth="1"/>
+    <col min="3" max="3" width="31.41796875" customWidth="1"/>
+    <col min="4" max="4" width="13.15625" customWidth="1"/>
+    <col min="5" max="5" width="10.83984375" customWidth="1"/>
+    <col min="6" max="6" width="8.68359375" customWidth="1"/>
+    <col min="7" max="7" width="18.15625" customWidth="1"/>
+    <col min="8" max="8" width="8.83984375" customWidth="1"/>
+    <col min="9" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="1" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="2" spans="2:8" ht="14.25" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -3204,106 +3402,106 @@
         <v>34968</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:8" ht="14.25" customHeight="1">
+      <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="4">
-        <v>8742.0</v>
-      </c>
-      <c r="E3" s="16">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
+        <v>8742</v>
+      </c>
+      <c r="E3" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="14.25" customHeight="1">
       <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="2:8" ht="14.25" customHeight="1">
       <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="2:8" ht="14.25" customHeight="1">
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="2:8" ht="14.25" customHeight="1">
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="2:8" ht="14.25" customHeight="1">
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" ht="14.25" customHeight="1">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="14.25" customHeight="1">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.25" customHeight="1">
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:8" ht="14.25" customHeight="1">
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:8" ht="14.25" customHeight="1">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="C29" s="19"/>
-    </row>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="16" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="17" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="3:3" ht="14.25" customHeight="1">
+      <c r="C29" s="17"/>
+    </row>
+    <row r="30" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="3:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -4273,36 +4471,34 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="22.29"/>
-    <col customWidth="1" min="3" max="3" width="45.57"/>
-    <col customWidth="1" min="4" max="4" width="24.71"/>
-    <col customWidth="1" min="5" max="5" width="31.86"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
-    <col customWidth="1" min="7" max="7" width="16.14"/>
-    <col customWidth="1" min="8" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="22.26171875" customWidth="1"/>
+    <col min="3" max="3" width="45.578125" customWidth="1"/>
+    <col min="4" max="4" width="24.68359375" customWidth="1"/>
+    <col min="5" max="5" width="31.83984375" customWidth="1"/>
+    <col min="6" max="6" width="8.68359375" customWidth="1"/>
+    <col min="7" max="7" width="16.15625" customWidth="1"/>
+    <col min="8" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="1" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="2" spans="2:8" ht="14.25" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -4323,7 +4519,7 @@
         <v>6330</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="2:8" ht="14.25" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>20</v>
       </c>
@@ -4331,80 +4527,80 @@
         <v>21</v>
       </c>
       <c r="D3" s="4">
-        <v>1055.0</v>
-      </c>
-      <c r="E3" s="17">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
+        <v>1055</v>
+      </c>
+      <c r="E3" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="14.25" customHeight="1">
       <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="2:8" ht="14.25" customHeight="1">
       <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="2:8" ht="14.25" customHeight="1">
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="2:8" ht="14.25" customHeight="1">
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="2:8" ht="14.25" customHeight="1">
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" ht="14.25" customHeight="1">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="14.25" customHeight="1">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.25" customHeight="1">
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:8" ht="14.25" customHeight="1">
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:8" ht="14.25" customHeight="1">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="16" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -5390,37 +5586,35 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="19.29"/>
-    <col customWidth="1" min="3" max="3" width="22.57"/>
-    <col customWidth="1" min="4" max="4" width="19.57"/>
-    <col customWidth="1" min="5" max="5" width="22.86"/>
-    <col customWidth="1" min="6" max="6" width="15.43"/>
-    <col customWidth="1" min="7" max="7" width="20.57"/>
-    <col customWidth="1" min="8" max="8" width="33.14"/>
-    <col customWidth="1" min="9" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="19.26171875" customWidth="1"/>
+    <col min="3" max="3" width="22.578125" customWidth="1"/>
+    <col min="4" max="4" width="19.578125" customWidth="1"/>
+    <col min="5" max="5" width="22.83984375" customWidth="1"/>
+    <col min="6" max="6" width="15.41796875" customWidth="1"/>
+    <col min="7" max="7" width="20.578125" customWidth="1"/>
+    <col min="8" max="8" width="33.15625" customWidth="1"/>
+    <col min="9" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="1" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="2" spans="2:8" ht="14.25" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -5441,7 +5635,7 @@
         <v>20900</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="2:8" ht="14.25" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
@@ -5449,91 +5643,91 @@
         <v>23</v>
       </c>
       <c r="D3" s="4">
-        <v>6100.0</v>
-      </c>
-      <c r="E3" s="17">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="B4" s="15" t="s">
+        <v>6100</v>
+      </c>
+      <c r="E3" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="14.25" customHeight="1">
+      <c r="B4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="20">
-        <v>2600.0</v>
-      </c>
-      <c r="E4" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="F4" s="21" t="s">
+      <c r="D4" s="4">
+        <v>2600</v>
+      </c>
+      <c r="E4" s="15">
+        <v>1</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="2:8" ht="14.25" customHeight="1">
       <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="2:8" ht="14.25" customHeight="1">
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="2:8" ht="14.25" customHeight="1">
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="2:8" ht="14.25" customHeight="1">
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" ht="14.25" customHeight="1">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="14.25" customHeight="1">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.25" customHeight="1">
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:8" ht="14.25" customHeight="1">
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:8" ht="14.25" customHeight="1">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="16" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -6520,39 +6714,39 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F4"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="23.14"/>
-    <col customWidth="1" min="3" max="3" width="22.43"/>
-    <col customWidth="1" min="4" max="4" width="23.71"/>
-    <col customWidth="1" min="5" max="5" width="31.57"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
-    <col customWidth="1" min="7" max="7" width="22.0"/>
-    <col customWidth="1" min="8" max="8" width="32.43"/>
-    <col customWidth="1" min="9" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="38.62890625" customWidth="1"/>
+    <col min="3" max="3" width="27.15625" customWidth="1"/>
+    <col min="4" max="4" width="23.68359375" customWidth="1"/>
+    <col min="5" max="5" width="31.578125" customWidth="1"/>
+    <col min="6" max="6" width="8.68359375" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="32.41796875" customWidth="1"/>
+    <col min="9" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="1" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="2" spans="2:8" ht="14.25" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -6569,84 +6763,59 @@
         <v>17</v>
       </c>
       <c r="H2" s="14">
-        <f t="array" ref="H2">SUM(D3:D201*E3:E201)</f>
+        <f t="array" ref="H2">SUM(D8:D201*E8:E201)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="B3" s="6"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="17"/>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="B4" s="6"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="B5" s="6"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="B6" s="6"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="3" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="4" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="5" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="6" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="7" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="8" spans="2:8" ht="14.25" customHeight="1">
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" ht="14.25" customHeight="1">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="14.25" customHeight="1">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.25" customHeight="1">
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:8" ht="14.25" customHeight="1">
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:8" ht="14.25" customHeight="1">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="16" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -7632,36 +7801,34 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="16.14"/>
-    <col customWidth="1" min="3" max="3" width="22.86"/>
-    <col customWidth="1" min="4" max="4" width="24.57"/>
-    <col customWidth="1" min="5" max="5" width="29.57"/>
-    <col customWidth="1" min="6" max="6" width="19.71"/>
-    <col customWidth="1" min="7" max="8" width="15.57"/>
-    <col customWidth="1" min="9" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="16.15625" customWidth="1"/>
+    <col min="3" max="3" width="22.83984375" customWidth="1"/>
+    <col min="4" max="4" width="24.578125" customWidth="1"/>
+    <col min="5" max="5" width="29.578125" customWidth="1"/>
+    <col min="6" max="6" width="19.68359375" customWidth="1"/>
+    <col min="7" max="8" width="15.578125" customWidth="1"/>
+    <col min="9" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="1" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="2" spans="2:8" ht="14.25" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -7671,7 +7838,7 @@
       <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="13" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="14" t="s">
@@ -7682,309 +7849,309 @@
         <v>14974.8</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="2:8" ht="14.25" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="20">
-        <v>10.0</v>
-      </c>
-      <c r="E3" s="16">
-        <v>900.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="B4" s="15" t="s">
+      <c r="D3" s="4">
+        <v>10</v>
+      </c>
+      <c r="E3" s="15">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="14.25" customHeight="1">
+      <c r="B4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="4">
         <v>5.4</v>
       </c>
-      <c r="E4" s="16">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="B5" s="15" t="s">
+      <c r="E4" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="14.25" customHeight="1">
+      <c r="B5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="4">
         <v>1.73</v>
       </c>
-      <c r="E5" s="23">
-        <v>3360.0</v>
-      </c>
-      <c r="F5" s="21" t="s">
+      <c r="E5" s="15">
+        <v>3360</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="2:8" ht="14.25" customHeight="1">
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="2:8" ht="14.25" customHeight="1">
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="2:8" ht="14.25" customHeight="1">
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" ht="14.25" customHeight="1">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="14.25" customHeight="1">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.25" customHeight="1">
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:8" ht="14.25" customHeight="1">
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:8" ht="14.25" customHeight="1">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="C22" s="24" t="s">
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="16" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="17" spans="2:5" ht="14.25" customHeight="1"/>
+    <row r="18" spans="2:5" ht="14.25" customHeight="1"/>
+    <row r="19" spans="2:5" ht="14.25" customHeight="1"/>
+    <row r="20" spans="2:5" ht="14.25" customHeight="1"/>
+    <row r="21" spans="2:5" ht="14.25" customHeight="1"/>
+    <row r="22" spans="2:5" ht="14.25" customHeight="1">
+      <c r="C22" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="C23" s="25" t="s">
+    <row r="23" spans="2:5" ht="14.25" customHeight="1">
+      <c r="C23" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="25">
-        <v>270.0</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="C24" s="25" t="s">
+      <c r="D23" s="20">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="14.25" customHeight="1">
+      <c r="C24" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="20">
         <f>2*D23 + 10</f>
         <v>550</v>
       </c>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="C25" s="25" t="s">
+    <row r="25" spans="2:5" ht="14.25" customHeight="1">
+      <c r="C25" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="20">
         <f>D24*2 + 20</f>
         <v>1120</v>
       </c>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="C26" s="25" t="s">
+    <row r="26" spans="2:5" ht="14.25" customHeight="1">
+      <c r="C26" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D26" s="19">
         <f>3*D25</f>
         <v>3360</v>
       </c>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-    </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="C28" s="24" t="s">
+    <row r="27" spans="2:5" ht="14.25" customHeight="1">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+    </row>
+    <row r="28" spans="2:5" ht="14.25" customHeight="1">
+      <c r="C28" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D28" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="B29" s="26"/>
-      <c r="C29" s="28" t="s">
+    <row r="29" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B29" s="20"/>
+      <c r="C29" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="24">
-        <v>30.0</v>
-      </c>
-      <c r="E29" s="26"/>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="B30" s="26"/>
-      <c r="E30" s="26"/>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="B31" s="26"/>
-      <c r="C31" s="24" t="s">
+      <c r="D29" s="19">
+        <v>30</v>
+      </c>
+      <c r="E29" s="20"/>
+    </row>
+    <row r="30" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B30" s="20"/>
+      <c r="E30" s="20"/>
+    </row>
+    <row r="31" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B31" s="20"/>
+      <c r="C31" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="26"/>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="B32" s="26"/>
-      <c r="C32" s="25" t="s">
+      <c r="E31" s="20"/>
+    </row>
+    <row r="32" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B32" s="20"/>
+      <c r="C32" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="25">
-        <v>120.0</v>
-      </c>
-      <c r="E32" s="26"/>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="B33" s="26"/>
-      <c r="C33" s="25" t="s">
+      <c r="D32" s="20">
+        <v>120</v>
+      </c>
+      <c r="E32" s="20"/>
+    </row>
+    <row r="33" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B33" s="20"/>
+      <c r="C33" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="25">
-        <v>110.0</v>
-      </c>
-      <c r="E33" s="26"/>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="B34" s="26"/>
-      <c r="C34" s="25" t="s">
+      <c r="D33" s="20">
+        <v>110</v>
+      </c>
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B34" s="20"/>
+      <c r="C34" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="25">
-        <v>220.0</v>
-      </c>
-      <c r="E34" s="26"/>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="B35" s="26"/>
-      <c r="C35" s="25" t="s">
+      <c r="D34" s="20">
+        <v>220</v>
+      </c>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B35" s="20"/>
+      <c r="C35" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="25">
-        <v>120.0</v>
-      </c>
-      <c r="E35" s="26"/>
-    </row>
-    <row r="36" ht="14.25" customHeight="1">
-      <c r="B36" s="26"/>
-      <c r="C36" s="25" t="s">
+      <c r="D35" s="20">
+        <v>120</v>
+      </c>
+      <c r="E35" s="20"/>
+    </row>
+    <row r="36" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B36" s="20"/>
+      <c r="C36" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="25">
-        <v>220.0</v>
-      </c>
-      <c r="E36" s="26"/>
-    </row>
-    <row r="37" ht="14.25" customHeight="1">
-      <c r="B37" s="26"/>
-      <c r="C37" s="25" t="s">
+      <c r="D36" s="20">
+        <v>220</v>
+      </c>
+      <c r="E36" s="20"/>
+    </row>
+    <row r="37" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B37" s="20"/>
+      <c r="C37" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="25">
-        <v>5.0</v>
-      </c>
-      <c r="E37" s="26"/>
-    </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="B38" s="26"/>
-      <c r="C38" s="25" t="s">
+      <c r="D37" s="20">
+        <v>5</v>
+      </c>
+      <c r="E37" s="20"/>
+    </row>
+    <row r="38" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B38" s="20"/>
+      <c r="C38" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="25">
-        <v>100.0</v>
-      </c>
-      <c r="E38" s="26"/>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="B39" s="26"/>
-      <c r="C39" s="25" t="s">
+      <c r="D38" s="20">
+        <v>100</v>
+      </c>
+      <c r="E38" s="20"/>
+    </row>
+    <row r="39" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B39" s="20"/>
+      <c r="C39" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="27">
+      <c r="D39" s="19">
         <f>SUM(D32:D38)</f>
         <v>895</v>
       </c>
-      <c r="E39" s="26"/>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="B40" s="26"/>
-      <c r="E40" s="26"/>
-    </row>
-    <row r="41" ht="14.25" customHeight="1">
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-    </row>
-    <row r="42" ht="14.25" customHeight="1">
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-    </row>
-    <row r="43" ht="14.25" customHeight="1">
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-    </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-    </row>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+      <c r="E39" s="20"/>
+    </row>
+    <row r="40" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B40" s="20"/>
+      <c r="E40" s="20"/>
+    </row>
+    <row r="41" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+    </row>
+    <row r="42" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+    </row>
+    <row r="43" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+    </row>
+    <row r="44" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+    </row>
+    <row r="45" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+    </row>
+    <row r="46" spans="2:5" ht="14.25" customHeight="1"/>
+    <row r="47" spans="2:5" ht="14.25" customHeight="1"/>
+    <row r="48" spans="2:5" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -8939,39 +9106,37 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F5"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="19.43"/>
-    <col customWidth="1" min="3" max="3" width="30.29"/>
-    <col customWidth="1" min="4" max="4" width="18.14"/>
-    <col customWidth="1" min="5" max="5" width="23.86"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
-    <col customWidth="1" min="7" max="7" width="20.71"/>
-    <col customWidth="1" min="8" max="8" width="26.29"/>
-    <col customWidth="1" min="9" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="19.41796875" customWidth="1"/>
+    <col min="3" max="3" width="30.26171875" customWidth="1"/>
+    <col min="4" max="4" width="18.15625" customWidth="1"/>
+    <col min="5" max="5" width="23.83984375" customWidth="1"/>
+    <col min="6" max="6" width="8.68359375" customWidth="1"/>
+    <col min="7" max="7" width="20.68359375" customWidth="1"/>
+    <col min="8" max="8" width="26.26171875" customWidth="1"/>
+    <col min="9" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="1" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="2" spans="2:8" ht="14.25" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -8992,7 +9157,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="2:8" ht="14.25" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>51</v>
       </c>
@@ -9000,80 +9165,80 @@
         <v>52</v>
       </c>
       <c r="D3" s="4">
-        <v>2400.0</v>
-      </c>
-      <c r="E3" s="17">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
+        <v>2400</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="14.25" customHeight="1">
       <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="2:8" ht="14.25" customHeight="1">
       <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="2:8" ht="14.25" customHeight="1">
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="2:8" ht="14.25" customHeight="1">
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="2:8" ht="14.25" customHeight="1">
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" ht="14.25" customHeight="1">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="14.25" customHeight="1">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.25" customHeight="1">
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:8" ht="14.25" customHeight="1">
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:8" ht="14.25" customHeight="1">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="16" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -10059,36 +10224,34 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="24.57"/>
-    <col customWidth="1" min="3" max="4" width="18.86"/>
-    <col customWidth="1" min="5" max="5" width="21.14"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
-    <col customWidth="1" min="7" max="7" width="19.43"/>
-    <col customWidth="1" min="8" max="8" width="19.29"/>
-    <col customWidth="1" min="9" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="24.578125" customWidth="1"/>
+    <col min="3" max="4" width="18.83984375" customWidth="1"/>
+    <col min="5" max="5" width="21.15625" customWidth="1"/>
+    <col min="6" max="6" width="8.68359375" customWidth="1"/>
+    <col min="7" max="7" width="19.41796875" customWidth="1"/>
+    <col min="8" max="8" width="19.26171875" customWidth="1"/>
+    <col min="9" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="1" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="2" spans="2:8" ht="14.25" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -10109,80 +10272,80 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="2:8" ht="14.25" customHeight="1">
       <c r="B3" s="6"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="17"/>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="2:8" ht="14.25" customHeight="1">
       <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="2:8" ht="14.25" customHeight="1">
       <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="2:8" ht="14.25" customHeight="1">
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="2:8" ht="14.25" customHeight="1">
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="2:8" ht="14.25" customHeight="1">
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" ht="14.25" customHeight="1">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="14.25" customHeight="1">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.25" customHeight="1">
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:8" ht="14.25" customHeight="1">
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:8" ht="14.25" customHeight="1">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="16" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -11168,37 +11331,37 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="19.14"/>
-    <col customWidth="1" min="3" max="3" width="24.57"/>
-    <col customWidth="1" min="4" max="4" width="19.0"/>
-    <col customWidth="1" min="5" max="5" width="17.0"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
-    <col customWidth="1" min="7" max="7" width="24.43"/>
-    <col customWidth="1" min="8" max="8" width="29.71"/>
-    <col customWidth="1" min="9" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.68359375" customWidth="1"/>
+    <col min="2" max="2" width="19.15625" customWidth="1"/>
+    <col min="3" max="3" width="24.578125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="8.68359375" customWidth="1"/>
+    <col min="7" max="7" width="24.41796875" customWidth="1"/>
+    <col min="8" max="8" width="29.68359375" customWidth="1"/>
+    <col min="9" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="1" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="2" spans="2:8" ht="14.25" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -11219,7 +11382,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="2:8" ht="14.25" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>53</v>
       </c>
@@ -11227,127 +11390,127 @@
         <v>54</v>
       </c>
       <c r="D3" s="4">
-        <v>150.0</v>
-      </c>
-      <c r="E3" s="16">
-        <v>48.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
+        <v>150</v>
+      </c>
+      <c r="E3" s="15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="14.25" customHeight="1">
       <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="2:8" ht="14.25" customHeight="1">
       <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="2:8" ht="14.25" customHeight="1">
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="2:8" ht="14.25" customHeight="1">
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="2:8" ht="14.25" customHeight="1">
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" ht="14.25" customHeight="1">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="14.25" customHeight="1">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.25" customHeight="1">
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:8" ht="14.25" customHeight="1">
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:8" ht="14.25" customHeight="1">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="C22" s="24" t="s">
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="16" spans="2:8" ht="14.25" customHeight="1"/>
+    <row r="17" spans="3:4" ht="14.25" customHeight="1"/>
+    <row r="18" spans="3:4" ht="14.25" customHeight="1"/>
+    <row r="19" spans="3:4" ht="14.25" customHeight="1"/>
+    <row r="20" spans="3:4" ht="14.25" customHeight="1"/>
+    <row r="21" spans="3:4" ht="14.25" customHeight="1"/>
+    <row r="22" spans="3:4" ht="14.25" customHeight="1">
+      <c r="C22" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="24"/>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="C23" s="25" t="s">
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="3:4" ht="14.25" customHeight="1">
+      <c r="C23" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="25">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="C24" s="25" t="s">
+      <c r="D23" s="20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" ht="14.25" customHeight="1">
+      <c r="C24" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="20">
         <f>2*D23</f>
         <v>24</v>
       </c>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="C25" s="25" t="s">
+    <row r="25" spans="3:4" ht="14.25" customHeight="1">
+      <c r="C25" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="19">
         <f>D24*2</f>
         <v>48</v>
       </c>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="C26" s="25"/>
-      <c r="D26" s="27"/>
-    </row>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="26" spans="3:4" ht="14.25" customHeight="1">
+      <c r="C26" s="20"/>
+      <c r="D26" s="19"/>
+    </row>
+    <row r="27" spans="3:4" ht="14.25" customHeight="1"/>
+    <row r="28" spans="3:4" ht="14.25" customHeight="1"/>
+    <row r="29" spans="3:4" ht="14.25" customHeight="1"/>
+    <row r="30" spans="3:4" ht="14.25" customHeight="1"/>
+    <row r="31" spans="3:4" ht="14.25" customHeight="1"/>
+    <row r="32" spans="3:4" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -12317,9 +12480,7 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>